<commit_message>
Updated Salaries and Tasks
</commit_message>
<xml_diff>
--- a/Salary/W10 Salaries and Tasks.xlsx
+++ b/Salary/W10 Salaries and Tasks.xlsx
@@ -1,23 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\feita\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Polybox Lokal\5.HS20\[W] HCI (Human Computer Interaction)\Übungen\0. Salaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995C9481-FE03-41B0-9896-1F45C42EC8DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21945" windowHeight="8085" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -36,21 +45,6 @@
   </si>
   <si>
     <t>Total Number of Team Members</t>
-  </si>
-  <si>
-    <t>Member 1</t>
-  </si>
-  <si>
-    <t>Member 2</t>
-  </si>
-  <si>
-    <t>Member 3</t>
-  </si>
-  <si>
-    <t>Member 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Member 5 </t>
   </si>
   <si>
     <t xml:space="preserve">Total salary distributed </t>
@@ -152,11 +146,38 @@
 Verify accuracy of all information.</t>
     </r>
   </si>
+  <si>
+    <t>Limette</t>
+  </si>
+  <si>
+    <t>Lukas Hasler</t>
+  </si>
+  <si>
+    <t>Pascal Strebel</t>
+  </si>
+  <si>
+    <t>Cedric Weibel</t>
+  </si>
+  <si>
+    <t>Robin Schmidiger</t>
+  </si>
+  <si>
+    <t>Added more parts to the frontend</t>
+  </si>
+  <si>
+    <t>Worked on our UI Library</t>
+  </si>
+  <si>
+    <t>Finish development of the frontend.</t>
+  </si>
+  <si>
+    <t>Start building the backend.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -277,9 +298,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -301,9 +319,12 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -580,154 +601,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.125" customWidth="1"/>
     <col min="2" max="2" width="34.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="90.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="10"/>
+      <c r="A1" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="10"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="11">
+        <v>44154</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="7"/>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="7"/>
+      <c r="B5" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="3"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="B8" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="7"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="7"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="7" t="s">
+      <c r="B14" s="7">
+        <f>SUM(B8:B12)</f>
+        <v>400</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="7"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="7"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B14" s="8">
-        <f>SUM(B8:B12)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <f>B5*100-B14</f>
         <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:2" ht="66" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>13</v>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" spans="1:2" ht="39" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
-      <c r="B19" s="7"/>
+      <c r="A19" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="7"/>
+      <c r="A20" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="7"/>
+      <c r="A21" s="6"/>
+      <c r="B21" s="6"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="7"/>
+      <c r="A22" s="6"/>
+      <c r="B22" s="6"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="7"/>
+      <c r="A23" s="6"/>
+      <c r="B23" s="6"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
+      <c r="A24" s="6"/>
+      <c r="B24" s="6"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
+      <c r="A25" s="6"/>
+      <c r="B25" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>